<commit_message>
Add examples and comments for api col
</commit_message>
<xml_diff>
--- a/examples/xlsx/accounting.xlsx
+++ b/examples/xlsx/accounting.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\edit-xlsx\examples\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\edit-xlsx\examples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6215D262-1070-4B1E-8EA0-42CED8060BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="25824" windowHeight="13896"/>
   </bookViews>
   <sheets>
     <sheet name="worksheet" sheetId="1" r:id="rId1"/>
@@ -113,7 +112,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +198,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -222,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +257,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -277,6 +284,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -550,37 +562,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="M1" sqref="M1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" customWidth="1"/>
-    <col min="3" max="12" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="3" max="12" width="12.77734375" customWidth="1"/>
+    <col min="13" max="14" width="8.77734375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-    </row>
-    <row r="2" spans="1:12" ht="28.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -594,53 +607,57 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" s="2" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9"/>
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="20"/>
+      <c r="G4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="17" t="s">
+      <c r="J4" s="20"/>
+      <c r="K4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="17"/>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="19"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3" t="s">
@@ -673,8 +690,10 @@
       <c r="L5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -682,7 +701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -690,7 +709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>20</v>
       </c>
@@ -698,7 +717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>21</v>
       </c>
@@ -706,7 +725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>30</v>
       </c>
@@ -714,7 +733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>31</v>
       </c>
@@ -722,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>40</v>
       </c>
@@ -730,7 +749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>41</v>
       </c>
@@ -738,7 +757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>50</v>
       </c>
@@ -746,7 +765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>51</v>
       </c>
@@ -754,7 +773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -814,52 +833,52 @@
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -876,9 +895,9 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A19" r:id="rId1" display="https://www.smartsheet.com/try-it?trp=8552&amp;lx=0I4W32CkGUrZg_vExFbzkQ&amp;utm_source=integrated+content&amp;utm_campaign=/top-excel-accounting-templates&amp;utm_medium=accounting+journal+template" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A20" r:id="rId2" display="https://www.smartsheet.com/try-it?trp=8552&amp;lx=0I4W32CkGUrZg_vExFbzkQ&amp;utm_source=integrated+content&amp;utm_campaign=/top-excel-accounting-templates&amp;utm_medium=accounting+journal+template" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A21" r:id="rId3" display="https://www.smartsheet.com/try-it?trp=8552&amp;lx=0I4W32CkGUrZg_vExFbzkQ&amp;utm_source=integrated+content&amp;utm_campaign=/top-excel-accounting-templates&amp;utm_medium=accounting+journal+template" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A19" r:id="rId1" display="https://www.smartsheet.com/try-it?trp=8552&amp;lx=0I4W32CkGUrZg_vExFbzkQ&amp;utm_source=integrated+content&amp;utm_campaign=/top-excel-accounting-templates&amp;utm_medium=accounting+journal+template"/>
+    <hyperlink ref="A20" r:id="rId2" display="https://www.smartsheet.com/try-it?trp=8552&amp;lx=0I4W32CkGUrZg_vExFbzkQ&amp;utm_source=integrated+content&amp;utm_campaign=/top-excel-accounting-templates&amp;utm_medium=accounting+journal+template"/>
+    <hyperlink ref="A21" r:id="rId3" display="https://www.smartsheet.com/try-it?trp=8552&amp;lx=0I4W32CkGUrZg_vExFbzkQ&amp;utm_source=integrated+content&amp;utm_campaign=/top-excel-accounting-templates&amp;utm_medium=accounting+journal+template"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>

</xml_diff>